<commit_message>
New file created called: csv_converter.py that converts all the xlsm files into csv files for ease of database integration in workbench. Also some code modifications occured in etl.py
</commit_message>
<xml_diff>
--- a/Temizlenmiş Üye Bilgi Liste/Temizlenmiş Üye Bilgi Liste - 1. komite.xlsx
+++ b/Temizlenmiş Üye Bilgi Liste/Temizlenmiş Üye Bilgi Liste - 1. komite.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J365"/>
+  <dimension ref="A1:I365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,11 +441,10 @@
     <col width="14" customWidth="1" min="3" max="3"/>
     <col width="62" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
-    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="24" customWidth="1" min="6" max="6"/>
     <col width="24" customWidth="1" min="7" max="7"/>
     <col width="129" customWidth="1" min="8" max="8"/>
     <col width="108" customWidth="1" min="9" max="9"/>
-    <col width="29" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -476,7 +475,7 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Meslek Grubu Sayı</t>
+          <t>Meslek Grubu Numarası</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -492,11 +491,6 @@
       <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Tescilli Adresi</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Meslek Grubu</t>
         </is>
       </c>
     </row>
@@ -542,11 +536,6 @@
           <t>HALKAPINAR MAHALLESİ 1490 SOKAK NO:3 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -590,11 +579,6 @@
           <t>MANSUROĞLU MAH. ANKARA CAD. NO: 81 İÇ KAPI NO: 148 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -638,11 +622,6 @@
           <t>ATATÜRK MAHALLESİ 2179 SK. NO: 2B URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J4" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -686,11 +665,6 @@
           <t>ADALET MAH. MANAS BUL. FOLKART TOWERS NO: 47B İÇ KAPI NO: 2601 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J5" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -734,11 +708,6 @@
           <t>GÜLBAHÇE MAHALLESİ 12080 NO:23 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -782,11 +751,6 @@
           <t>TUNA MAHALLESİ ŞEHİT ÜSTEĞMEN AHMET KONUKSEVER SOKAK NO:3 KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J7" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -830,11 +794,6 @@
           <t>ADALET MAH. 1586/3 SK. NO: 40 İÇ KAPI NO: 7 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J8" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -878,11 +837,6 @@
           <t>ÇINARLI MAH. ANKARA ASFALTI CAD. NO: 15 İÇ KAPI NO: 451 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J9" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -926,11 +880,6 @@
           <t>ADALET MAHALLESİ 1586/3 SOK. NO: 40 İÇ KAPI NO: 4 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J10" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -974,11 +923,6 @@
           <t>KAZIMDİRİK MAHALLESİ 367 SOK. NO: 3-5 İÇ KAPI NO: 414 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J11" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1022,11 +966,6 @@
           <t>EGEMENLİK MAH. 6106/15 SK. NO: 5A BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J12" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1070,11 +1009,6 @@
           <t>ÇAMBEL MAH. ANKARA CAD. NO: 341/2 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J13" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1118,11 +1052,6 @@
           <t>KAZIMDİRİK MAHALLESİ 296/2 SOKAK NO:33 3.SANAYİ SİTESİ BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J14" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -1166,11 +1095,6 @@
           <t>AOSB MAH. M. KEMAL ATATÜRK BUL. NO: 21 ÇİĞLİ / İZMİR</t>
         </is>
       </c>
-      <c r="J15" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1214,11 +1138,6 @@
           <t>AKDENİZ MAHALLESİ 1329 SOKAK NO:20/603 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J16" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -1262,11 +1181,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. KAYNAKLAR BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J17" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1310,11 +1224,6 @@
           <t>BASIN SİTESİ MAHALLESİ GAZETECİ HASAN TAHSİN CD. NURİYE APT. Apt. NO: 129 KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J18" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -1358,11 +1267,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/G103 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J19" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -1406,11 +1310,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239V İÇ KAPI NO: 26 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J20" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -1454,11 +1353,6 @@
           <t>AKDENİZ MAH. GAZİ OSMAN PAŞA BUL. SÜREYYA REYENT İŞHAN NO: 30 İÇ KAPI NO: 608 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J21" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -1502,11 +1396,6 @@
           <t>CELAL BAYAR MAHALLESİ 5152 SOK. NO:9 ÇEŞME / İZMİR</t>
         </is>
       </c>
-      <c r="J22" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -1550,11 +1439,6 @@
           <t>ÇINARLI MAH. ŞEHİT POLİS FETHİ SEKİN CAD. NO: 1 İÇ KAPI NO: 1101 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J23" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -1598,11 +1482,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 G/100 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J24" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -1646,11 +1525,6 @@
           <t>TEPECİK MAHALLESİ KUŞADASI CAD. NO: 79B SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J25" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -1694,11 +1568,6 @@
           <t>İNÖNÜ MAHALLESİ 672 SK. NO: 114A BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J26" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -1742,11 +1611,6 @@
           <t>OSMANGAZİ MAHALLESİ 592/1 SOK. NO:3 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J27" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -1790,11 +1654,6 @@
           <t>TURABİYE MAH. NECAT HEPKON CAD. NO: 46 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J28" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -1838,11 +1697,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239G İÇ KAPI NO: 101 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J29" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -1886,11 +1740,6 @@
           <t>FATİH MAH. 1191 SK. NO: 5/6 GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J30" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -1934,11 +1783,6 @@
           <t>BOSTANLI MAHALLESİ 1779 SK. NO: 4 /1A KARŞIYAKA/İZMİR</t>
         </is>
       </c>
-      <c r="J31" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1982,11 +1826,6 @@
           <t>TORASAN MAH. PINARDERE SK. NO: 21 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J32" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -2030,11 +1869,6 @@
           <t>İSMET KAPTAN MAH. ŞEHİT NEVRES BUL. DEREN PLAZA BLOK NO: 10 İÇ KAPI NO: 11 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J33" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -2078,11 +1912,6 @@
           <t>ZAFER MAHALLESİ 2347 SK. NO:11 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J34" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -2126,11 +1955,6 @@
           <t>KEMALPAŞA OSB MAH. İZMİR ANKARA CAD. NO: 67 İÇ KAPI NO: 1 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J35" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -2174,11 +1998,6 @@
           <t>YILDIZ MAH. 206/28 SK. NO: 3 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J36" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -2222,11 +2041,6 @@
           <t>ADALET MAH. MANAS BUL. FOLKART TOWERS NO: 39 İÇ KAPI NO: 3408 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J37" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -2270,11 +2084,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 P/48 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J38" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -2318,11 +2127,6 @@
           <t>ÇOLAK İBRAHİM BEY MAHALLESİ FEVZİ ÇAKMAK CAD. NO:2 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J39" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -2366,11 +2170,6 @@
           <t>ÇAMÖNÜ MAH. 21 SK. NO: 11 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J40" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -2414,11 +2213,6 @@
           <t>ÇOLAK İBRAHİM BEY MAH. FEVZİ ÇAKMAK CAD. NO: 2 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J41" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -2462,11 +2256,6 @@
           <t>KASIMPAŞA MAH. 201/1 SK. NO: 4C MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J42" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -2510,11 +2299,6 @@
           <t>SEKİZ EYLÜL MAHALLESİ 5012 SK. NO:226/1 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J43" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -2558,11 +2342,6 @@
           <t>SOĞUKPINAR MAHALLESİ ATATÜRK BULVARI NO: 12 İÇ KAPI NO: 9 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J44" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -2606,11 +2385,6 @@
           <t>İSMET KAPTAN MAHALLESİ 1367 SOKAK İSMET KAPTAN MAH. 1367 SK. YAZGILI İŞ MERKEZİ KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J45" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -2654,11 +2428,6 @@
           <t>YENİKALE MAHALLESİ İSMAİL CEM SOK. NO:4/19 NARLIDERE / İZMİR</t>
         </is>
       </c>
-      <c r="J46" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -2702,11 +2471,6 @@
           <t>EGEMENLİK MAHALLESİ 6108 SOKAK KARA NAK.SİTESİ F BLOK NO: 51/10B BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J47" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -2750,11 +2514,6 @@
           <t>KALABAK MAH. 3031 SK. NO: 4 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J48" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -2798,11 +2557,6 @@
           <t>TEPECİK MAHALLESİ KAVAKDERE CD. NO:60 SEFERİHİSAR/İZMİR</t>
         </is>
       </c>
-      <c r="J49" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -2846,11 +2600,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239P İÇ KAPI NO: 44 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J50" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
@@ -2894,11 +2643,6 @@
           <t>İSMET KAPTAN MAH. 1369 SK. TANAÇAN BLOK NO: 40 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J51" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -2942,11 +2686,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239V İÇ KAPI NO: 8 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J52" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -2990,11 +2729,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239C İÇ KAPI NO: 4 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J53" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -3038,11 +2772,6 @@
           <t>FATİH MAHALLESİ 1209 SOK. NO:2 GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J54" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
@@ -3086,11 +2815,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J55" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
@@ -3134,11 +2858,6 @@
           <t>MİMAR SİNAN MAHALLESİ MİMAR SİNAN CAD. NO:27/5 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J56" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
@@ -3182,11 +2901,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239G/112-239H/112A KAYNAKLAR BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J57" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
@@ -3230,11 +2944,6 @@
           <t>ADALET MAHALLESİ 1586/1 NO:NO:1/B/K:2 D:6 BAYRAKLI/İZMİR</t>
         </is>
       </c>
-      <c r="J58" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
@@ -3278,11 +2987,6 @@
           <t>KAZIMDİRİK MAHALLESİ 296/2 SOKAK NO:33 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J59" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
@@ -3326,11 +3030,6 @@
           <t>HÜRRİYET MAHALLESİ AYDERESİ SULUK KÜME EVLERİ NO:4/B ARMUTLU KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J60" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
@@ -3374,11 +3073,6 @@
           <t>ADALET MAHALLESİ MANAS BULV. FOLKART TOWERS BLOK NO: 47B İÇ KAPI NO: 260 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J61" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
@@ -3422,11 +3116,6 @@
           <t>KÖYİÇİ MAHALLESİ ATATÜRK SK. NO:7 SALMAN KÖYÜ KARABURUN / İZMİR</t>
         </is>
       </c>
-      <c r="J62" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -3470,11 +3159,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 C/16 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J63" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
@@ -3518,11 +3202,6 @@
           <t>FİKRİ ALTAY MAHALLESİ ANADOLU CADDESİ NO:541 KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J64" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
@@ -3566,11 +3245,6 @@
           <t>AKDENİZ MAH. CUMHURİYET BUL. ERDEN İŞ HANI BLOK NO: 87 İÇ KAPI NO: 12 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J65" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
@@ -3614,11 +3288,6 @@
           <t>TORASAN MAHALLESİ PINARDERE SK. NO: 43/ URLA/İZMİR</t>
         </is>
       </c>
-      <c r="J66" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
@@ -3662,11 +3331,6 @@
           <t>ADALET MAHALLESİ MANAS BULVARI NO:47/B FOLKART TOWERS BLOK İÇ KAPI NO: 2601 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J67" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
@@ -3710,11 +3374,6 @@
           <t>YENİKENT MAHALLESİ EMEK SK. İZLEMEK-YAŞAM SİTESİ İZLEMEK-YAŞAM BLOK URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J68" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
@@ -3758,11 +3417,6 @@
           <t>HALKAPINAR MAH. 1203 SK. NO: 13 İÇ KAPI NO: 724 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J69" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
@@ -3806,11 +3460,6 @@
           <t>ADATEPE MAH. DOĞUŞ CAD. NO: 207AG İÇ KAPI NO: 1 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J70" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
@@ -3854,11 +3503,6 @@
           <t>İÇMELER MAHALLESİ 1154 SK. NO:10 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J71" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
@@ -3902,11 +3546,6 @@
           <t>KÜLTÜR MAHALLESİ ŞEHİT NEVRES BULVARI NO:5/8-9 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J72" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
@@ -3950,11 +3589,6 @@
           <t>ADALET MAHALLESİ MANAS BLV. FOLKART TOWERS APT. NO: 47 B/2809 BAYRAKLI/İZMİR</t>
         </is>
       </c>
-      <c r="J73" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
@@ -3998,11 +3632,6 @@
           <t>GAZİ MAH. 28/25 NO:NO:11/A GAZİEMİR/İZMİR</t>
         </is>
       </c>
-      <c r="J74" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
@@ -4046,11 +3675,6 @@
           <t>ATATÜRK MAHALLESİ 29 EKİM CADDESİ NO: 239G İÇ KAPI NO: 107 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J75" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
@@ -4094,11 +3718,6 @@
           <t>MANSUROĞLU MAHALLESİ 286/2 SOK. NO:2/15 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J76" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
@@ -4142,11 +3761,6 @@
           <t>KÜLTÜR MAH. DR. MUSTAFA ENVER BEY CAD. BERKİ APT BLOK NO: 1/1 İÇ KAPI NO: 81 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J77" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -4190,11 +3804,6 @@
           <t>KOCATEPE MAH. 574/1 SK. NO: 4 İÇ KAPI NO: 5 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J78" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
@@ -4238,11 +3847,6 @@
           <t>KAZIM DİRİK MAHALLESİ 375 SOK. NO:18 KAT:2 DAİRE:205 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J79" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
@@ -4286,11 +3890,6 @@
           <t>TEPECİK MAHALLESİ NO:34 KUŞADASI YOLU ÜZERİ SEFERİHİSAR/İZMİR</t>
         </is>
       </c>
-      <c r="J80" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
@@ -4334,11 +3933,6 @@
           <t>İNÖNÜ MAHALLESİ 672/10 SK. NO:28/A BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J81" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
@@ -4382,11 +3976,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239V İÇ KAPI NO: 18 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J82" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
@@ -4430,11 +4019,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 G/98 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J83" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
@@ -4478,11 +4062,6 @@
           <t>MANSUROĞLU MAHALLESİ 288/4 SOK. NO: 9/1 İÇ KAPI NO: 43 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J84" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
@@ -4526,11 +4105,6 @@
           <t>MANSUROĞLU MAH. 286/1 SK. NO: 1 İÇ KAPI NO: 215 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J85" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
@@ -4574,11 +4148,6 @@
           <t>İSMET KAPTAN MAHALLESİ 9 EYLÜL MEYDANI HÜDAVERDİ İŞ MERKEZİ BLOK NO: 3 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J86" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
@@ -4622,11 +4191,6 @@
           <t>YAYLACIK MAHALLESİ 178 SK. NO:10/10 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J87" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
@@ -4670,11 +4234,6 @@
           <t>BAHÇELİEVLER MAH. HALİDE EDİP ADIVAR CAD. NO: 14 İÇ KAPI NO: 15 KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J88" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
@@ -4718,11 +4277,6 @@
           <t>ÇOLAK İBRAHİM BEY MAH. FEVZİ ÇAKMAK CAD. NO: 2 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J89" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
@@ -4766,11 +4320,6 @@
           <t>ADALET MAHALLESİ MANAS FOLKART TOWERS BLOK NO: 47B İÇ KAPI NO: 26 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J90" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
@@ -4814,11 +4363,6 @@
           <t>SARIYER MAH. COŞKUN KALE SK. NO: 100A KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J91" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
@@ -4862,11 +4406,6 @@
           <t>ADALET MAHALLESİ MANAS BLV. NO: 39 İÇ KAPI NO: 3408 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J92" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
@@ -4910,11 +4449,6 @@
           <t>AŞAĞIKIZILCA MAHALLESİ AŞAĞIKIZILCA OVA EVLERİ YOLU (KÜME EVLER) NO: 1/1A İÇ KAPI NO: 1 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J93" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
@@ -4958,11 +4492,6 @@
           <t>KAVAKLIDERE MAHALLESİ ÇITAK SOKAK NO:12/1 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J94" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
@@ -5006,11 +4535,6 @@
           <t>GÖRECE CUMHURİYET MAH. CEMAL GÜRSEL BUL. NO: 8 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J95" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
@@ -5054,11 +4578,6 @@
           <t>6219 SK. NO:11 GÜMÜLDÜR FEVZİ ÇAKMAK MAH. İÇ KAPI NO: 2 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J96" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
@@ -5102,11 +4621,6 @@
           <t>ZAFER MAHALLESİ 2373 SOKAK NO:9 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J97" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
@@ -5150,11 +4664,6 @@
           <t>SELVİLİ MAHALLESİ 4139 SK. NO: 29 A/A KARABAĞLAR/İZMİR</t>
         </is>
       </c>
-      <c r="J98" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
@@ -5198,11 +4707,6 @@
           <t>SARILAR MAHALLESİ NO:177 SAZ MAH.YOLU KÜME EVLERİ 18738316 SİTESİ KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J99" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
@@ -5246,11 +4750,6 @@
           <t>YAKAKÖY MAH. POLİGON SK. NO: 38/1 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J100" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
@@ -5294,11 +4793,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 P/54 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J101" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
@@ -5342,11 +4836,6 @@
           <t>SEKİZ EYLÜL MAH. 113 SK. NO: 16 İÇ KAPI NO: 8 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J102" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
@@ -5390,11 +4879,6 @@
           <t>ÖZBEK MAHALLESİ 6217 SK. NO: 29 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J103" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
@@ -5438,11 +4922,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239C İÇ KAPI NO: 24 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J104" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
@@ -5486,11 +4965,6 @@
           <t>KAZIMDİRİK MAHALLESİ 161 SOKAK NO:11/D BORNOVA/İZMİR</t>
         </is>
       </c>
-      <c r="J105" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
@@ -5534,11 +5008,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 G/96 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J106" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
@@ -5582,11 +5051,6 @@
           <t>AKSOY MAHALLESİ 1746 SK. GÜLTEKİN Apt. NO: 4/2 KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J107" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
@@ -5630,11 +5094,6 @@
           <t>SOĞUKPINAR MAHALLESİ SOĞUKPINAR (KÜME EVLER) NO:47 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J108" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
@@ -5678,11 +5137,6 @@
           <t>KAVAKLIDERE MAH. ÇITAK SK. NO: 12/1 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J109" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
@@ -5726,11 +5180,6 @@
           <t>HALKAPINAR MAHALLESİ 1203/11 SOKAK K.HASAN ATLI İŞMERK. BLOK NO: 4/630 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J110" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
@@ -5774,11 +5223,6 @@
           <t>ONUR MAH. 7370 SK. NO: 15 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J111" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
@@ -5822,11 +5266,6 @@
           <t>KONAK MAHALLESİ ÇOBANOĞLU ZEKİ BEY CADDESİ NO:7/204 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J112" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
@@ -5870,11 +5309,6 @@
           <t>BAYRAKLI MAHALLESİ ORD. PROF. DR. EKREM AKURGAL SK. HAFİZE HANIM APT. NO: 85 A BAYRAKLI/İZMİR</t>
         </is>
       </c>
-      <c r="J113" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
@@ -5918,11 +5352,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/C-12 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J114" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
@@ -5966,11 +5395,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/ZH BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J115" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
@@ -6014,11 +5438,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 G/101 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J116" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
@@ -6062,11 +5481,6 @@
           <t>İSKELE MAHALLESİ HALİL ALTUN CADDESİ NO:23/A AKVARYUM SİTESİ KARABURUN / İZMİR</t>
         </is>
       </c>
-      <c r="J117" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
@@ -6110,11 +5524,6 @@
           <t>TEPECİK MAHALLESİ KUŞADASI CAD. NO: 77 A/ SEFERİHİSAR/İZMİR</t>
         </is>
       </c>
-      <c r="J118" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
@@ -6158,11 +5567,6 @@
           <t>REİSDERE MAHALLESİ 6001 SOK. NO: 18A ÇEŞME / İZMİR</t>
         </is>
       </c>
-      <c r="J119" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
@@ -6206,11 +5610,6 @@
           <t>ÖRNEKKÖY MAH. 1001 SK. NO: 19 İÇ KAPI NO: 4 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J120" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
@@ -6254,11 +5653,6 @@
           <t>ADALET MAHALLESİ MANAS BLV. NO: 47 B/2601 BAYRAKLI/İZMİR</t>
         </is>
       </c>
-      <c r="J121" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
@@ -6302,11 +5696,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 P/43 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J122" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
@@ -6350,11 +5739,6 @@
           <t>SEKİZ EYLÜL MAHALLESİ 111 SOKAK NO: 13 İÇ KAPI NO: 1 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J123" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
@@ -6398,11 +5782,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 G/82 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J124" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
@@ -6446,11 +5825,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/G76 KAYNAKLAR BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J125" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
@@ -6494,11 +5868,6 @@
           <t>TEPEKULE MAH. 2084/7 SK. SEYHANKENT SİTESİ DİLARA BLOK NO: 17B BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J126" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
@@ -6542,11 +5911,6 @@
           <t>KAZIMDİRİK MAH. 296/2 SK. NO: 33 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J127" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
@@ -6590,11 +5954,6 @@
           <t>ÜMİT MAH. 1411/4 SK. NO: 15E BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J128" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
@@ -6638,11 +5997,6 @@
           <t>ATATÜRK MAHALLESİ İSTİKBAL CAD. NO: 165/1 GÜZELBAHÇE/İZMİR</t>
         </is>
       </c>
-      <c r="J129" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
@@ -6686,11 +6040,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239G İÇ KAPI NO: 90 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J130" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
@@ -6734,11 +6083,6 @@
           <t>MİMAR SİNAN MAH. 1394 SK. CENK NO: 16D İÇ KAPI NO: 16D KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J131" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
@@ -6782,11 +6126,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/V15 KAYNAKLAR BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J132" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
@@ -6830,11 +6169,6 @@
           <t>YENİ MAHALLESİ ZAFER CAD. NO:26 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J133" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
@@ -6878,11 +6212,6 @@
           <t>ATIFBEY MAHALLESİ 2. NO:14/A B BLOK Apt. GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J134" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
@@ -6926,11 +6255,6 @@
           <t>MERİÇ MAHALLESİ KEMALPAŞA CAD. NO:46 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J135" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
@@ -6974,11 +6298,6 @@
           <t>BAHRİYE ÜÇOK MAHALLESİ 1762 SK. NO: 9 İÇ KAPI NO: 1 KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J136" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
@@ -7022,11 +6341,6 @@
           <t>GÜVENDİK MAHALLESİ 136 SK. NO:45/A/0 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J137" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
@@ -7070,11 +6384,6 @@
           <t>EĞİTİM MAH. ZİYA GÖKALP SK. NO: 93 İÇ KAPI NO: 1 BALÇOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J138" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
@@ -7118,11 +6427,6 @@
           <t>MERSİNLİ MAH. 2816 SK. NO: 86A KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J139" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
@@ -7166,11 +6470,6 @@
           <t>KONAK MAHALLESİ MİLLİ KÜTÜPHANE CADDESİ BARÇIN SPOR MAĞAZASI BLOK NO: 27 İÇKAPINO:Z1 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J140" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
@@ -7214,11 +6513,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. KAYNAKLAR BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J141" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
@@ -7262,11 +6556,6 @@
           <t>FEVZİ ÇAKMAK MAHALLESİ 4006 SOKAK NO:3 ALAÇATI ÇEŞME / İZMİR</t>
         </is>
       </c>
-      <c r="J142" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
@@ -7310,11 +6599,6 @@
           <t>ADALET MAHALLESİ MANAS BLV. FOLKART TOWERS APT. NO: 47 B/2601 BAYRAKLI/İZMİR</t>
         </is>
       </c>
-      <c r="J143" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
@@ -7358,11 +6642,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/V-16 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J144" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
@@ -7406,11 +6685,6 @@
           <t>EGEMENLİK MAHALLESİ 6153 SK. NO: 4S BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J145" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
@@ -7454,11 +6728,6 @@
           <t>YILDIRIM BEYAZIT MAHALLESİ YILDIRIM BEYAZIT CAD. NO: 50 A BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J146" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
@@ -7502,11 +6771,6 @@
           <t>MERSİNLİ MAHALLESİ 2823/1 SK. NO: 4 İÇ KAPI NO: Z12 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J147" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
@@ -7550,11 +6814,6 @@
           <t>ZAFER MAH. TURGUT ÖZAL CAD. NO: 20 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J148" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
@@ -7598,11 +6857,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 V/32 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J149" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
@@ -7646,11 +6900,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 P/37 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J150" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
@@ -7694,11 +6943,6 @@
           <t>EGEMENLİK MAHALLESİ 6112 SOKAK TİCARET MERKEZİ Apt. NO: 1/125 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J151" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
@@ -7742,11 +6986,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/E-15 KAYNAKLAR BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J152" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
@@ -7790,11 +7029,6 @@
           <t>ATATÜRK MAHALLESİ 2176 SK. NO:16 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J153" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
@@ -7838,11 +7072,6 @@
           <t>KONAK MAHALLESİ CUMHURİYET BLV. KAPANİ İŞ MERKEZİ BLOK NO: 36 İÇKAPI NO:711 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J154" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
@@ -7886,11 +7115,6 @@
           <t>ÇİÇEKLİ MAHALLESİ PINARLI SK. NO: 24 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J155" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
@@ -7934,11 +7158,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/19 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J156" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
@@ -7982,11 +7201,6 @@
           <t>ADALET MAHALLESİ MANAS BLV. FOLKART TOWERS Apt. NO: 39/3208 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J157" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
@@ -8030,11 +7244,6 @@
           <t>EVKA 3 MAH. 121 SK. NO: 42/1G İÇ KAPI NO: 1 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J158" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
@@ -8078,11 +7287,6 @@
           <t>SOĞUKPINAR MAH. 300 SK. NO: 12B KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J159" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
@@ -8126,11 +7330,6 @@
           <t>DEVELİ MAHALLESİ ÇEVRE YOLU BLV. NO:195 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J160" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
@@ -8174,11 +7373,6 @@
           <t>İÇMELER MAHALLESİ ESKİ URLA-İZMİR YOLU CAD. NO: 20 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J161" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
@@ -8222,11 +7416,6 @@
           <t>TURGUT REİS MAH. ŞEHİT NİHATBEY CAD. NO: 115 İÇ KAPI NO: 10 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J162" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
@@ -8270,11 +7459,6 @@
           <t>BOSTANLI MAH. DR. ZİYA ERTEMER SK. NO: 5A KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J163" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
@@ -8318,11 +7502,6 @@
           <t>SELVİLİ MAHALLESİ 4019/5 SK. AFYON BLOK NO: 4A KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J164" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
@@ -8366,11 +7545,6 @@
           <t>KÜLTÜR MAHALLESİ MUSTAFA MÜNİR BİRSEL SK. NO: 4 /1/103 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J165" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
@@ -8414,11 +7588,6 @@
           <t>ADALET MAH. MANAS BUL. FOLKART TOWERS BLOK NO: 47B İÇ KAPI NO: 3509 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J166" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
@@ -8462,11 +7631,6 @@
           <t>MUSALLA MAHALLESİ PAFTA:28-H ADA:472 PARSEL:98 ÇEŞME / İZMİR</t>
         </is>
       </c>
-      <c r="J167" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
@@ -8510,11 +7674,6 @@
           <t>MİTHATPAŞA MAH. OVA YOLU SK. NO: 48A MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J168" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
@@ -8558,11 +7717,6 @@
           <t>GÜMÜLDÜR ATATÜRK MAHALLESİ GÜMÜLDÜR İZMİR CAD. NO:271 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J169" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
@@ -8606,11 +7760,6 @@
           <t>RAFET PAŞA MAH. 5178 SK. NO: 22 İÇ KAPI NO: 1 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J170" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
@@ -8654,11 +7803,6 @@
           <t>GÜRPINAR MAH. 7004/3 SK. NO: 13/5 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J171" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
@@ -8702,11 +7846,6 @@
           <t>TEPECİK MAHALLESİ 118 SOK. NO:1 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J172" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
@@ -8750,11 +7889,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239E İÇ KAPI NO: 27 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J173" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
@@ -8798,11 +7932,6 @@
           <t>VALİ RAHMİ BEY MAH. FORBES SK. YILMAZ BLOK NO: 123 İÇ KAPI NO: 7 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J174" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
@@ -8846,11 +7975,6 @@
           <t>GÜMÜLDÜR CUMHURİYET MAHALLESİ TEMELPAŞA CAD. NO: 56 -2/-2 MENDERES/İZMİR</t>
         </is>
       </c>
-      <c r="J175" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
@@ -8894,11 +8018,6 @@
           <t>FİKRİ ALTAY MAHALLESİ ORDU BLV. NO: 168 A KARŞIYAKA/İZMİR</t>
         </is>
       </c>
-      <c r="J176" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
@@ -8942,11 +8061,6 @@
           <t>2.İNÖNÜ MAHALLESİ ALTINVADİ CAD. NO: 99 İÇ KAPI NO: 16 NARLIDERE / İZMİR</t>
         </is>
       </c>
-      <c r="J177" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="n">
@@ -8990,11 +8104,6 @@
           <t>GAZİ MAH. 26 SK. NO: 62 İÇ KAPI NO: 2 GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J178" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="179">
       <c r="A179" s="2" t="n">
@@ -9038,11 +8147,6 @@
           <t>BALATÇIK MAHALLESİ 8914 SK. NO: 75 A ÇİĞLİ / İZMİR</t>
         </is>
       </c>
-      <c r="J179" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="n">
@@ -9086,11 +8190,6 @@
           <t>CUMHURİYET MAH. KARAKOÇ CAD. NO: 84 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J180" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="n">
@@ -9134,11 +8233,6 @@
           <t>HÜRRİYET MAHALLESİ 1087 SK. NO: 5 /A//A GAZİEMİR/İZMİR</t>
         </is>
       </c>
-      <c r="J181" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
@@ -9182,11 +8276,6 @@
           <t>AKDENİZ MAH. 1353 SK. TANER İŞHANI NO: 1 İÇ KAPI NO: 608 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J182" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
@@ -9230,11 +8319,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/E-25 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J183" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
@@ -9278,11 +8362,6 @@
           <t>GAZİ MAHALLESİ 28/30 SK. ZİRAAT BANKASI APT. NO: 18/1 GAZİEMİR/İZMİR</t>
         </is>
       </c>
-      <c r="J184" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="185">
       <c r="A185" s="2" t="n">
@@ -9326,11 +8405,6 @@
           <t>ADALET MAHALLESİ MANAS BLV. NO:39/3408 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J185" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="n">
@@ -9374,11 +8448,6 @@
           <t>HUZUR MAHALLESİ AÇELYAM SOKAK A BLOK NO: 7 İÇ KAPI NO: 10 NARLIDERE / İZMİR</t>
         </is>
       </c>
-      <c r="J186" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="187">
       <c r="A187" s="2" t="n">
@@ -9422,11 +8491,6 @@
           <t>ÖRNEKKÖY MAHALLESİ ÖRNEKKÖY (KÜME EVLER) NO:24/1 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J187" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
@@ -9470,11 +8534,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239 P/52 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J188" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="189">
       <c r="A189" s="2" t="n">
@@ -9518,11 +8577,6 @@
           <t>YENİKALE MAH. FIRAT SK. NO: 2 İÇ KAPI NO: 3 NARLIDERE / İZMİR</t>
         </is>
       </c>
-      <c r="J189" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
@@ -9566,11 +8620,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 C/12 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J190" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="191">
       <c r="A191" s="2" t="n">
@@ -9614,11 +8663,6 @@
           <t>KONAK MAH. 859 SK. SARAY İŞHANI BLOK NO: 5 İÇ KAPI NO: 506 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J191" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="n">
@@ -9662,11 +8706,6 @@
           <t>ALSANCAK MAH. KIBRIS ŞEHİTLERİ CAD. İŞÇİMENLER İŞ MERKEZİ NO: 146 İÇ KAPI NO: 9 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J192" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="193">
       <c r="A193" s="2" t="n">
@@ -9710,11 +8749,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J193" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="194">
       <c r="A194" s="2" t="n">
@@ -9758,11 +8792,6 @@
           <t>NARLI MAHALLESİ ŞENCAN SK. PELİN BLOK NO: 15A NARLIDERE / İZMİR</t>
         </is>
       </c>
-      <c r="J194" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="195">
       <c r="A195" s="2" t="n">
@@ -9806,11 +8835,6 @@
           <t>ÇAMÖNÜ MAH. 17/1 SK. NO: 25/1 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J195" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="196">
       <c r="A196" s="2" t="n">
@@ -9854,11 +8878,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 P/35 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J196" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="197">
       <c r="A197" s="2" t="n">
@@ -9902,11 +8921,6 @@
           <t>TELEFERİK MAHALLESİ AKÇAKAYA (KÜME EVLER) H.KABAKCI Apt. NO: 19/1 BALÇOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J197" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="198">
       <c r="A198" s="2" t="n">
@@ -9950,11 +8964,6 @@
           <t>UĞUR MUMCU MAH. 8790/11 SK. NO: 2 ÇİĞLİ / İZMİR</t>
         </is>
       </c>
-      <c r="J198" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="199">
       <c r="A199" s="2" t="n">
@@ -9998,11 +9007,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 G/105 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J199" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="200">
       <c r="A200" s="2" t="n">
@@ -10046,11 +9050,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 P/41 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J200" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="201">
       <c r="A201" s="2" t="n">
@@ -10094,11 +9093,6 @@
           <t>MEHMET AKİF ERSOY MAHALLESİ KİRAZLI CD. NO:134/1 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J201" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="202">
       <c r="A202" s="2" t="n">
@@ -10142,11 +9136,6 @@
           <t>MEHMET AKİF ERSOY MAHALLESİ KİRAZLI CD. NO: 132 A KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J202" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="203">
       <c r="A203" s="2" t="n">
@@ -10190,11 +9179,6 @@
           <t>NALDÖKEN MAHALLESİ 1273/1 SK. NO: 2 C BORNOVA/İZMİR</t>
         </is>
       </c>
-      <c r="J203" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="204">
       <c r="A204" s="2" t="n">
@@ -10238,11 +9222,6 @@
           <t>ERZENE MAH. GENÇLİK CAD. NO: 11 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J204" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="205">
       <c r="A205" s="2" t="n">
@@ -10286,11 +9265,6 @@
           <t>YEŞİLOVA MAHALLESİ 4016 SOKAK ATIFBEY SİTESİ 2 BLOK NO: 8 İÇ KAPI NO: 19 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J205" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="206">
       <c r="A206" s="2" t="n">
@@ -10334,11 +9308,6 @@
           <t>DOKUZ EYLÜL MAH. 692 SK. NO: 16 GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J206" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="207">
       <c r="A207" s="2" t="n">
@@ -10382,11 +9351,6 @@
           <t>AHMETBEYLİ MAH. CLAROS BUL. NO: 506 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J207" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="208">
       <c r="A208" s="2" t="n">
@@ -10430,11 +9394,6 @@
           <t>HACI İSA MAH. ZAFER CAD. NO: 4 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J208" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="209">
       <c r="A209" s="2" t="n">
@@ -10478,11 +9437,6 @@
           <t>LİMANREİS MAH. MİTHATPAŞA CAD. NO: 606 NARLIDERE / İZMİR</t>
         </is>
       </c>
-      <c r="J209" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="210">
       <c r="A210" s="2" t="n">
@@ -10526,11 +9480,6 @@
           <t>ZAFER MAH. TURGUT ÖZAL CAD. NO: 6 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J210" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="211">
       <c r="A211" s="2" t="n">
@@ -10574,11 +9523,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD.239 G/110 - 239 H/110A NO:/ BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J211" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="212">
       <c r="A212" s="2" t="n">
@@ -10622,11 +9566,6 @@
           <t>ZAFER MAH. 2371 SK. NO: 7 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J212" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="213">
       <c r="A213" s="2" t="n">
@@ -10670,11 +9609,6 @@
           <t>PİRİ REİS MAHALLESİ 200 SOKAK KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J213" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="n">
@@ -10718,11 +9652,6 @@
           <t>FATİH MAH. 1191 SK. NO: 5/6 GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J214" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="215">
       <c r="A215" s="2" t="n">
@@ -10766,11 +9695,6 @@
           <t>ATİLLA MAHALLESİ 464 SOKAK NO: 73C İÇ KAPI NO: C KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J215" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="216">
       <c r="A216" s="2" t="n">
@@ -10814,11 +9738,6 @@
           <t>CUMHURİYET MAHALLESİ 6702 SK. NO:2 İÇ KAPI NO: 7 KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J216" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="217">
       <c r="A217" s="2" t="n">
@@ -10862,11 +9781,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 G/93 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J217" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="n">
@@ -10910,11 +9824,6 @@
           <t>ADALET MAH. 1593/13 SK. NO: 26 İÇ KAPI NO: 1 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J218" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="219">
       <c r="A219" s="2" t="n">
@@ -10958,11 +9867,6 @@
           <t>SALMAN MAH. ZEYTİNCİLER KÜME EVLERİ NO: 95 İÇ KAPI NO: 1 KARABURUN / İZMİR</t>
         </is>
       </c>
-      <c r="J219" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="220">
       <c r="A220" s="2" t="n">
@@ -11006,11 +9910,6 @@
           <t>KEMALPAŞA O.S.B. MAHALLESİ İZMİR ANKARA ASFALTI CD. NO:7-7/1</t>
         </is>
       </c>
-      <c r="J220" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="221">
       <c r="A221" s="2" t="n">
@@ -11054,11 +9953,6 @@
           <t>ÇINARLI MAHALLESİ 1572 SK. NO: 33/- KONAK/İZMİR</t>
         </is>
       </c>
-      <c r="J221" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="n">
@@ -11102,11 +9996,6 @@
           <t>KAZIMDİRİK MAH. 369/2 SK. NO: 1 İÇ KAPI NO: 93 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J222" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="223">
       <c r="A223" s="2" t="n">
@@ -11150,11 +10039,6 @@
           <t>ATIFBEY MAHALLESİ 67 SOKAK NO: 33 İÇ KAPI NO: 32 GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J223" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="224">
       <c r="A224" s="2" t="n">
@@ -11198,11 +10082,6 @@
           <t>HIDIRLIK MAHALLESİ TUZLA CADDESI NO:135 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J224" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="225">
       <c r="A225" s="2" t="n">
@@ -11246,11 +10125,6 @@
           <t>KONAK MAHALLESİ CUMHURİYET BLV. KONAK İŞHANI APT. NO: 24/56 KONAK/İZMİR</t>
         </is>
       </c>
-      <c r="J225" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="226">
       <c r="A226" s="2" t="n">
@@ -11294,11 +10168,6 @@
           <t>KEMALPAŞA MAHALLESİ 7415 SOKAK NO: 1 İÇ KAPI NO: Z1 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J226" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="227">
       <c r="A227" s="2" t="n">
@@ -11342,11 +10211,6 @@
           <t>ADALET MAHALLESİ ANADOLU CADDESİ NO:41/101 MEGAPOL TOWER BLOK BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J227" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="228">
       <c r="A228" s="2" t="n">
@@ -11390,11 +10254,6 @@
           <t>MUSTAFA KEMAL MAHALLESİ 6753/1 SOKAK NO:2/7 DAİRE:14 KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J228" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="229">
       <c r="A229" s="2" t="n">
@@ -11438,11 +10297,6 @@
           <t>YELKİ MAH. İNÖNÜ CAD. NO: 28 İÇ KAPI NO: 3 GÜZELBAHÇE / İZMİR</t>
         </is>
       </c>
-      <c r="J229" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="230">
       <c r="A230" s="2" t="n">
@@ -11486,11 +10340,6 @@
           <t>DOKUZ EYLÜL MAHALLESİ ÖNDER CAD. NO: 38/205 GAZİEMİR/İZMİR</t>
         </is>
       </c>
-      <c r="J230" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="231">
       <c r="A231" s="2" t="n">
@@ -11534,11 +10383,6 @@
           <t>ZAFER MAH. 2330 SK. NO: 6A BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J231" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="232">
       <c r="A232" s="2" t="n">
@@ -11582,11 +10426,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239G İÇ KAPI NO: 77 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J232" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="n">
@@ -11630,11 +10469,6 @@
           <t>ALSANCAK MAHALLESİ MAHMUT ESAT BOZKURT CAD. ERAY APT. NO: 29 B KONAK/İZMİR</t>
         </is>
       </c>
-      <c r="J233" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="234">
       <c r="A234" s="2" t="n">
@@ -11678,11 +10512,6 @@
           <t>ZAFER MAHALLESİ 2342 SK. NO:4 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J234" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="235">
       <c r="A235" s="2" t="n">
@@ -11726,11 +10555,6 @@
           <t>ZAFER MAH. TURGUT ÖZAL CAD. NO: 110 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J235" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="236">
       <c r="A236" s="2" t="n">
@@ -11774,11 +10598,6 @@
           <t>İHSAN ALYANAK MAH. 4972 SK. NO: 21 İÇ KAPI NO: MÜSTAKİL KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J236" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="237">
       <c r="A237" s="2" t="n">
@@ -11822,11 +10641,6 @@
           <t>ADALET MAH. MANAS BUL. NO: 39 İÇ KAPI NO: 2511 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J237" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="238">
       <c r="A238" s="2" t="n">
@@ -11870,11 +10684,6 @@
           <t>ADALET MAH. MANAS BUL. FOLKART TOWERS NO: 47B İÇ KAPI NO: 2601 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J238" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="239">
       <c r="A239" s="2" t="n">
@@ -11918,11 +10727,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239P İÇ KAPI NO: 50 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J239" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="240">
       <c r="A240" s="2" t="n">
@@ -11966,11 +10770,6 @@
           <t>BAHÇELİEVLER MAHALLESİ 1853/3 SK. NO: 2 B KARŞIYAKA/İZMİR</t>
         </is>
       </c>
-      <c r="J240" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="241">
       <c r="A241" s="2" t="n">
@@ -12014,11 +10813,6 @@
           <t>29 EKİM MAH. 2190 SK. NO: 13A BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J241" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="242">
       <c r="A242" s="2" t="n">
@@ -12062,11 +10856,6 @@
           <t>BİNBAŞI REŞAT BEY MAHALLESİ 351/1 SOKAK NO:14/A GAZİEMİR/İZMİR</t>
         </is>
       </c>
-      <c r="J242" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="243">
       <c r="A243" s="2" t="n">
@@ -12110,11 +10899,6 @@
           <t>BASIN SİTESİ MAHALLESİ 169 SOKAK NO:19/8 KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J243" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="244">
       <c r="A244" s="2" t="n">
@@ -12158,11 +10942,6 @@
           <t>ERZENE MAH. ANKARA CAD. EBİLTEM NO: 172/14 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J244" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="245">
       <c r="A245" s="2" t="n">
@@ -12206,11 +10985,6 @@
           <t>İTOB ORGANİZE SANAYİ BÖLGESİ TEKELİ MAHALLESİ 10001 SOKAK NO:9 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J245" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="246">
       <c r="A246" s="2" t="n">
@@ -12254,11 +11028,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239V İÇ KAPI NO: 21 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J246" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="247">
       <c r="A247" s="2" t="n">
@@ -12302,11 +11071,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239G/112-239H/112A KAYNAKLAR BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J247" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="248">
       <c r="A248" s="2" t="n">
@@ -12350,11 +11114,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/G İÇ KAPI NO: 84 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J248" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="249">
       <c r="A249" s="2" t="n">
@@ -12398,11 +11157,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/E-23 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J249" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="250">
       <c r="A250" s="2" t="n">
@@ -12446,11 +11200,6 @@
           <t>İNCİRALTI MAHALLESİ 8/9 SOKAK NO:58 BALÇOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J250" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="251">
       <c r="A251" s="2" t="n">
@@ -12494,11 +11243,6 @@
           <t>ALAÇATI MAHALLESİ 16032 SK. NO:81/B ÇEŞME / İZMİR</t>
         </is>
       </c>
-      <c r="J251" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="252">
       <c r="A252" s="2" t="n">
@@ -12542,11 +11286,6 @@
           <t>NO:47 KUŞÇULAR MAH. 8034 SK URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J252" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="253">
       <c r="A253" s="2" t="n">
@@ -12590,11 +11329,6 @@
           <t>ALİ FUAT ERDEN MAH. MAHALLESİ 9799. SOKAK NO:20/2 KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J253" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="254">
       <c r="A254" s="2" t="n">
@@ -12638,11 +11372,6 @@
           <t>ADALET MAHALLESİ ANADOLU CAD. MEGAPOL TOWER BLOK NO: 41 İÇ KAPI NO: 101 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J254" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="255">
       <c r="A255" s="2" t="n">
@@ -12686,11 +11415,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/95 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J255" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="256">
       <c r="A256" s="2" t="n">
@@ -12734,11 +11458,6 @@
           <t>MUSTAFA KEMAL MAHALLESİ BÜLENT ECEVİT CAD. NO:50/A/16 YÜKSEK VADİ EVLERİ Sit. KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J256" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="257">
       <c r="A257" s="2" t="n">
@@ -12782,11 +11501,6 @@
           <t>KAHRAMANLAR MAHALLESİ 1427 SOKAK NO: 10A İÇ KAPI NO: A KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J257" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="258">
       <c r="A258" s="2" t="n">
@@ -12830,11 +11544,6 @@
           <t>ÇINARLI MAHALLESİ OZAN ABAY CADDESİ NO:10/193 B Apt KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J258" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="259">
       <c r="A259" s="2" t="n">
@@ -12878,11 +11587,6 @@
           <t>KAHRAMANDERE MAH. ATA CAD. NO: 52 İÇ KAPI NO: 13 GÜZELBAHÇE / İZMİR</t>
         </is>
       </c>
-      <c r="J259" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="260">
       <c r="A260" s="2" t="n">
@@ -12926,11 +11630,6 @@
           <t>MANSUROĞLU MAH. 1593/1 SK. NO: 6 İÇ KAPI NO: 53 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J260" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="261">
       <c r="A261" s="2" t="n">
@@ -12974,11 +11673,6 @@
           <t>ADALET MAHALLESİ MANAS BULV. FOLKART TOWERS BLOK NO: 47B İÇ KAPI NO: 260 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J261" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="262">
       <c r="A262" s="2" t="n">
@@ -13022,11 +11716,6 @@
           <t>ADALET MAHALLESİ ANADOLU CADDESİ NO: 41/1 İÇ KAPI NO: 703 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J262" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="263">
       <c r="A263" s="2" t="n">
@@ -13070,11 +11759,6 @@
           <t>YALI MAHALLESİ MİTHATPAŞA CD. NO:110 GÜZELBAHÇE / İZMİR</t>
         </is>
       </c>
-      <c r="J263" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="264">
       <c r="A264" s="2" t="n">
@@ -13118,11 +11802,6 @@
           <t>ADALET MAHALLESİ MANAS BLV. NO: 12 /2 BAYRAKLI/İZMİR</t>
         </is>
       </c>
-      <c r="J264" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="265">
       <c r="A265" s="2" t="n">
@@ -13166,11 +11845,6 @@
           <t>ADALET MAH. MANAS BUL. FOLKART TOWERS NO: 47B İÇ KAPI NO: 2601 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J265" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="266">
       <c r="A266" s="2" t="n">
@@ -13214,11 +11888,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239G İÇ KAPI NO: 87 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J266" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="267">
       <c r="A267" s="2" t="n">
@@ -13262,11 +11931,6 @@
           <t>MALTEPE MAHALLESİ 110 SK. NO: 20/_ GÜZELBAHÇE/İZMİR</t>
         </is>
       </c>
-      <c r="J267" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="268">
       <c r="A268" s="2" t="n">
@@ -13310,11 +11974,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239G İÇ KAPI NO: 104 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J268" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="269">
       <c r="A269" s="2" t="n">
@@ -13358,11 +12017,6 @@
           <t>CAMİKEBİR MAH. 50 SOK NO:3A SEFERİHİSAR/İZMİR</t>
         </is>
       </c>
-      <c r="J269" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="270">
       <c r="A270" s="2" t="n">
@@ -13406,11 +12060,6 @@
           <t>GÜZELYURT MAHALLESİ 920 SOK. NO:50 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J270" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="271">
       <c r="A271" s="2" t="n">
@@ -13454,11 +12103,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/V14 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J271" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="272">
       <c r="A272" s="2" t="n">
@@ -13502,11 +12146,6 @@
           <t>KİBAR MAH. 3777 SK. NO: 4 İÇ KAPI NO: 3 KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J272" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="273">
       <c r="A273" s="2" t="n">
@@ -13550,11 +12189,6 @@
           <t>KORUTÜRK MAHALLESİ V. HÜSEYİN ÖĞÜTÇEN CAD. DİKMEN Apt. NO: 5 /A/7 BALÇOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J273" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="274">
       <c r="A274" s="2" t="n">
@@ -13598,11 +12232,6 @@
           <t>YILDIZ MAH. AHMET PİRİŞTİNA BUL. NO: 21 İÇ KAPI NO: 20 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J274" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="275">
       <c r="A275" s="2" t="n">
@@ -13646,11 +12275,6 @@
           <t>YEŞİLOVA MAHALLESİ 4045 SOKAK NO: 48A BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J275" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="276">
       <c r="A276" s="2" t="n">
@@ -13694,11 +12318,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239P İÇ KAPI NO: 38 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J276" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="277">
       <c r="A277" s="2" t="n">
@@ -13742,11 +12361,6 @@
           <t>KUŞÇULAR MAHALLESİ 8012 SOKAK NO:15 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J277" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="278">
       <c r="A278" s="2" t="n">
@@ -13790,11 +12404,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/V-33 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J278" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="279">
       <c r="A279" s="2" t="n">
@@ -13838,11 +12447,6 @@
           <t>YİĞİTLER MAH. YİĞİTLER YOLU KÜME EVLERİ 18372856 SİTESİ NO: 254 İÇ KAPI NO: 1 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J279" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="280">
       <c r="A280" s="2" t="n">
@@ -13886,11 +12490,6 @@
           <t>HIDIRLIK MAH. 78/2 SK. NO: 7H SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J280" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="281">
       <c r="A281" s="2" t="n">
@@ -13934,11 +12533,6 @@
           <t>HALKAPINAR MAH. 1203/11 SK. K.HASAN ATLI İŞMERK. BLOK NO: 4 İÇ KAPI NO: 630 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J281" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="282">
       <c r="A282" s="2" t="n">
@@ -13982,11 +12576,6 @@
           <t>YERALTI MAHALLESİ İNCİRLİ KÜME EVLERİ NO: 103 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J282" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="283">
       <c r="A283" s="2" t="n">
@@ -14030,11 +12619,6 @@
           <t>ERGENE MAHALLESİ MUSTAFA KEMAL CAD. ÇELİK Sit. B Apt. NO: 20 /1/5 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J283" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="284">
       <c r="A284" s="2" t="n">
@@ -14078,11 +12662,6 @@
           <t>MEHMET AKİF ERSOY MAH. DR. ALİ KARAMAN CAD. NO: 6A KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J284" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="285">
       <c r="A285" s="2" t="n">
@@ -14126,11 +12705,6 @@
           <t>İÇMELER MAHALLESİ ESKİ URLA-İZMİR YOLU CAD. NO: 36 İÇ KAPI NO: 1 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J285" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="286">
       <c r="A286" s="2" t="n">
@@ -14174,11 +12748,6 @@
           <t>İSMET KAPTAN MAH. ŞEHİT NEVRES BUL. DEREN PLAZA NO: 10 İÇ KAPI NO: 11 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J286" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="287">
       <c r="A287" s="2" t="n">
@@ -14222,11 +12791,6 @@
           <t>ZEYTİNLER MAH. GAZİ MUSTAFA KEMAL CAD. NO: 35A URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J287" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="288">
       <c r="A288" s="2" t="n">
@@ -14270,11 +12834,6 @@
           <t>CUMHURİYET MAHALLESİ İZMİR ANKARA ASFALTI 35. KM NO:200/A KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J288" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="289">
       <c r="A289" s="2" t="n">
@@ -14318,11 +12877,6 @@
           <t>ADALET MAHALLESİ MANAS BLV. FOLKART TOWERS BLOK NO:47B İÇ KAPI NO:2601 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J289" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="290">
       <c r="A290" s="2" t="n">
@@ -14366,11 +12920,6 @@
           <t>ZAFER MAHALLESİ 2360 SK. NO:49 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J290" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="291">
       <c r="A291" s="2" t="n">
@@ -14414,11 +12963,6 @@
           <t>HALKAPINAR MAHALLESİ 1082 SOKAK NO:3 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J291" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="292">
       <c r="A292" s="2" t="n">
@@ -14462,11 +13006,6 @@
           <t>MEHMET AKİF ERSOY MAH. SAYRA&amp;ÇINAR KÜME EVLERİ NO: 2 KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J292" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="293">
       <c r="A293" s="2" t="n">
@@ -14510,11 +13049,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/P DAİRE:46 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J293" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="294">
       <c r="A294" s="2" t="n">
@@ -14558,11 +13092,6 @@
           <t>GÜRPINAR MAHALLESİ 7232/8 SK. AY-KOOP SİT. NO: 39 A BORNOVA/İZMİR</t>
         </is>
       </c>
-      <c r="J294" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="295">
       <c r="A295" s="2" t="n">
@@ -14606,11 +13135,6 @@
           <t>CAMİKEBİR MAH. 52 SK. NO: 2 İÇ KAPI NO: 101 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J295" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="296">
       <c r="A296" s="2" t="n">
@@ -14654,11 +13178,6 @@
           <t>BAHRİYE ÜÇOK MAHALLESİ 1827 SK. NO:11/A GÜRAY BLOK KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J296" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="297">
       <c r="A297" s="2" t="n">
@@ -14702,11 +13221,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 ZL BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J297" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="298">
       <c r="A298" s="2" t="n">
@@ -14750,11 +13264,6 @@
           <t>KURUÇEŞME MAHALLESİ 205/17 SK. KESKİN BLOK NO: 31A BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J298" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="299">
       <c r="A299" s="2" t="n">
@@ -14798,11 +13307,6 @@
           <t>ALAYBEY MAH. ŞEHİT ASIM AKSOY CAD. AKTAN NO: 47A KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J299" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="300">
       <c r="A300" s="2" t="n">
@@ -14846,11 +13350,6 @@
           <t>BALATÇIK MAH. 8788/10 SK. B-BLOK NO: 5D ÇİĞLİ / İZMİR</t>
         </is>
       </c>
-      <c r="J300" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="301">
       <c r="A301" s="2" t="n">
@@ -14894,11 +13393,6 @@
           <t>BEYLER MAHALLESİ NO:46 SARILAR KÖYÜ KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J301" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="302">
       <c r="A302" s="2" t="n">
@@ -14942,11 +13436,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/P63 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J302" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="303">
       <c r="A303" s="2" t="n">
@@ -14990,11 +13479,6 @@
           <t>KAVAKLIDERE MAH. KAVAK SK. NO: 2 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J303" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="304">
       <c r="A304" s="2" t="n">
@@ -15038,11 +13522,6 @@
           <t>MANSUROĞLU MAHALLESİ 286/2 SOK. NO: 2/15 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J304" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="305">
       <c r="A305" s="2" t="n">
@@ -15086,11 +13565,6 @@
           <t>YAYLACIK MAHALLESİ BAŞARI CAD. NO:134/1 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J305" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="306">
       <c r="A306" s="2" t="n">
@@ -15134,11 +13608,6 @@
           <t>ADALET MAH. MANAS BUL. FOLKART TOWERS NO: 47B İÇ KAPI NO: 2601 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J306" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="307">
       <c r="A307" s="2" t="n">
@@ -15182,11 +13651,6 @@
           <t>MEHMET ALİ AKMAN MAHALLESİ 18/1 SOKAK NO:2/14 KONAK/İZMİR</t>
         </is>
       </c>
-      <c r="J307" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="308">
       <c r="A308" s="2" t="n">
@@ -15230,11 +13694,6 @@
           <t>ÇİLE MAHALLESİ 7457 SK. NO:14/1 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J308" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="309">
       <c r="A309" s="2" t="n">
@@ -15278,11 +13737,6 @@
           <t>ÇINARLI MAH. 1572 SK. NO: 33 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J309" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="310">
       <c r="A310" s="2" t="n">
@@ -15326,11 +13780,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239P İÇ KAPI NO: 49 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J310" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="311">
       <c r="A311" s="2" t="n">
@@ -15374,11 +13823,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 P/68 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J311" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="312">
       <c r="A312" s="2" t="n">
@@ -15422,11 +13866,6 @@
           <t>ADALET MAHALLESİ 1586/7 SOK. NO: 2 İÇ KAPI NO: 1 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J312" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="313">
       <c r="A313" s="2" t="n">
@@ -15470,11 +13909,6 @@
           <t>BALATÇIK MAH. 8900 SK. NO: 14A ÇİĞLİ / İZMİR</t>
         </is>
       </c>
-      <c r="J313" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="314">
       <c r="A314" s="2" t="n">
@@ -15518,11 +13952,6 @@
           <t>ADALET MAH. MANAS BUL. FOLKART TOWERS NO: 39 İÇ KAPI NO: 3201 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J314" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="315">
       <c r="A315" s="2" t="n">
@@ -15566,11 +13995,6 @@
           <t>ESENTEPE MAHALLESİ 14 SK. NO:103 KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J315" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="316">
       <c r="A316" s="2" t="n">
@@ -15614,11 +14038,6 @@
           <t>ALSANCAK MAHALLESİ 1479 SOKAK NO:16/2 KENET SİTESİ Apt. KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J316" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="317">
       <c r="A317" s="2" t="n">
@@ -15662,11 +14081,6 @@
           <t>EGEMENLİK MAHALLESİ 6153 SK. NO: 4 S/0 BORNOVA/İZMİR</t>
         </is>
       </c>
-      <c r="J317" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="318">
       <c r="A318" s="2" t="n">
@@ -15710,11 +14124,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO: 239 P/47 BUCA/İZMİR</t>
         </is>
       </c>
-      <c r="J318" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="319">
       <c r="A319" s="2" t="n">
@@ -15758,11 +14167,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J319" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="320">
       <c r="A320" s="2" t="n">
@@ -15806,11 +14210,6 @@
           <t>KEMALPAŞA MAHALLESİ 7087/3 SOKAK NO:1/3 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J320" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="321">
       <c r="A321" s="2" t="n">
@@ -15854,11 +14253,6 @@
           <t>YERALTI MAHALLESİ İNCİRLİ KÜME EVLERİ NO:96/O URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J321" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="322">
       <c r="A322" s="2" t="n">
@@ -15902,11 +14296,6 @@
           <t>GÜZELYALI MAHALLESİ MİTHATPAŞA CD. NO:917/12 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J322" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="323">
       <c r="A323" s="2" t="n">
@@ -15950,11 +14339,6 @@
           <t>ZEYBEK MAH. SELİMİYE CAD. NO: 40A KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J323" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="324">
       <c r="A324" s="2" t="n">
@@ -15998,11 +14382,6 @@
           <t>DUMLUPINAR MAHALLESİ 90 SK. NO:7/3 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J324" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="325">
       <c r="A325" s="2" t="n">
@@ -16046,11 +14425,6 @@
           <t>CÜNEYTBEY MAHALLESİ İBRAHİM TURAN CAD. NO: 8 İÇ KAPI NO: 2 MENDERES / İZMİR</t>
         </is>
       </c>
-      <c r="J325" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="326">
       <c r="A326" s="2" t="n">
@@ -16094,11 +14468,6 @@
           <t>GÖKSU MAHALLESİ 679 SK. NO: 23 İÇ KAPI NO: 1 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J326" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="327">
       <c r="A327" s="2" t="n">
@@ -16142,11 +14511,6 @@
           <t>SOĞUKKUYU MAH. 1847/14 SK. NO: 1 İÇ KAPI NO: 2 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J327" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="328">
       <c r="A328" s="2" t="n">
@@ -16190,11 +14554,6 @@
           <t>BAHÇELİEVLER MAH. ŞEHİT MUSTAFA TUNÇBİLEK SK. ALİ AĞA BLOK NO: 94A KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J328" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="329">
       <c r="A329" s="2" t="n">
@@ -16238,11 +14597,6 @@
           <t>BAHARİYE MAH. 1690 SK. NO: 148A KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J329" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="330">
       <c r="A330" s="2" t="n">
@@ -16286,11 +14640,6 @@
           <t>KAZIMDİRİK MAH. ÜNİVERSİTE CAD. ÖZGÖRKEY NO: 66 BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J330" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="331">
       <c r="A331" s="2" t="n">
@@ -16334,11 +14683,6 @@
           <t>KÜLTÜR MAHALLESİ CUMHURİYET BULVARI B BLOK NO: 141 İÇ KAPI NO: 1 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J331" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="332">
       <c r="A332" s="2" t="n">
@@ -16382,11 +14726,6 @@
           <t>ÇINARLI MAH. 1572 SK. NO: 33 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J332" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="333">
       <c r="A333" s="2" t="n">
@@ -16430,11 +14769,6 @@
           <t>NO:57/3 VATAN MAHALLESİ 9100 SK. KARABAĞLAR / İZMİR</t>
         </is>
       </c>
-      <c r="J333" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="334">
       <c r="A334" s="2" t="n">
@@ -16478,11 +14812,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239ZA BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J334" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="335">
       <c r="A335" s="2" t="n">
@@ -16526,11 +14855,6 @@
           <t>İNCİRALTI MAH. İNCİRALTI CAD. NO: 181 BALÇOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J335" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="336">
       <c r="A336" s="2" t="n">
@@ -16574,11 +14898,6 @@
           <t>TEPECİK MAHALLESİ KUŞADASI CAD. NO: 77 D/ SEFERİHİSAR/İZMİR</t>
         </is>
       </c>
-      <c r="J336" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="337">
       <c r="A337" s="2" t="n">
@@ -16622,11 +14941,6 @@
           <t>TEPECİK MAH. KUŞADASI CAD. UÇAK KARDEŞLER NO: 79 SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J337" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="338">
       <c r="A338" s="2" t="n">
@@ -16670,11 +14984,6 @@
           <t>ULUCAK MUSTAFA KEMAL ATATÜRK MAH. MEHMET AKİF ERSOY CAD. NO: 31B KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J338" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="339">
       <c r="A339" s="2" t="n">
@@ -16718,11 +15027,6 @@
           <t>YENİMAHALLE MAHALLESİ 8207 SK. NO: 11 A/0 ÇİĞLİ / İZMİR</t>
         </is>
       </c>
-      <c r="J339" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="340">
       <c r="A340" s="2" t="n">
@@ -16766,11 +15070,6 @@
           <t>HALKAPINAR MAHALLESİ 1203/11 SOKAK NO: 5-7 İÇ KAPI NO: 175 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J340" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="341">
       <c r="A341" s="2" t="n">
@@ -16814,11 +15113,6 @@
           <t>ATIFBEY MAHALLESİ FERİDUN PÖZÜT CAD. NO:40/A/A GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J341" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="342">
       <c r="A342" s="2" t="n">
@@ -16862,11 +15156,6 @@
           <t>DEDEBAŞI MAHALLESİ 1595 SK NO:225/405 KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J342" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="343">
       <c r="A343" s="2" t="n">
@@ -16910,11 +15199,6 @@
           <t>YALI MAHALLESİ 6323/1 SK. NO:18/E KARŞIYAKA / İZMİR</t>
         </is>
       </c>
-      <c r="J343" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="344">
       <c r="A344" s="2" t="n">
@@ -16958,11 +15242,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/V/12 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J344" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="345">
       <c r="A345" s="2" t="n">
@@ -17006,11 +15285,6 @@
           <t>KÜLTÜR MAH. MUSTAFA MÜNİR BİRSEL SK. KORDON İŞ HANI BLOK NO: 4/1 İÇ KAPI NO: 202 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J345" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="346">
       <c r="A346" s="2" t="n">
@@ -17054,11 +15328,6 @@
           <t>29 EKİM MAHALLESİ ATATÜRK CAD. NO:239/V 24 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J346" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="347">
       <c r="A347" s="2" t="n">
@@ -17102,11 +15371,6 @@
           <t>MANSUROĞLU MAHALLESİ 221 SOK. GÜLAY BLOK NO: 22A BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J347" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="348">
       <c r="A348" s="2" t="n">
@@ -17150,11 +15414,6 @@
           <t>ADALET MAH. MANAS BUL. NO: 39 İÇ KAPI NO: 3408 BAYRAKLI / İZMİR</t>
         </is>
       </c>
-      <c r="J348" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="349">
       <c r="A349" s="2" t="n">
@@ -17198,11 +15457,6 @@
           <t>AĞAÇÇEŞMESİ MEVKİİ MAHALLESİ NO:9 DÜZCE KÖYÜ AĞAÇEŞMESİ MEVKİİ SEFERİHİSAR/İZMİR</t>
         </is>
       </c>
-      <c r="J349" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="350">
       <c r="A350" s="2" t="n">
@@ -17246,11 +15500,6 @@
           <t>SEKİZ EYLÜL MAHALLESİ İZMİR CAD. NO: 103B KEMALPAŞA / İZMİR</t>
         </is>
       </c>
-      <c r="J350" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="351">
       <c r="A351" s="2" t="n">
@@ -17294,11 +15543,6 @@
           <t>GONCALAR MAHALLESİ 6007/7 SK. NO: 26 A KARŞIYAKA/İZMİR</t>
         </is>
       </c>
-      <c r="J351" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="352">
       <c r="A352" s="2" t="n">
@@ -17342,11 +15586,6 @@
           <t>İSMET KAPTAN MAHALLESİ 1385 SOKAK YENİ ASIR İŞ MERKEZİ BLOK NO: 3 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J352" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="353">
       <c r="A353" s="2" t="n">
@@ -17390,11 +15629,6 @@
           <t>KAHRAMANLAR MAHALLESİ EMRE ÖZDESTAN SK. NO:17/65 DEREN İŞ MRK. BLOK KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J353" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="354">
       <c r="A354" s="2" t="n">
@@ -17438,11 +15672,6 @@
           <t>YAKA MAH. ERDOĞAN KER CAD. NO: 77/71 URLA / İZMİR</t>
         </is>
       </c>
-      <c r="J354" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="355">
       <c r="A355" s="2" t="n">
@@ -17486,11 +15715,6 @@
           <t>KÜÇÜK ÇİĞLİ MAHALLESİ 8754/1 SOKAK NO:6/A ÇİĞLİ ÇİĞLİ / İZMİR</t>
         </is>
       </c>
-      <c r="J355" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="356">
       <c r="A356" s="2" t="n">
@@ -17534,11 +15758,6 @@
           <t>75.YIL CUMHURİYET MAHALLESİ NO:5 KARASULUK MEVKİİ KEMALPAŞA/İZMİR</t>
         </is>
       </c>
-      <c r="J356" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="357">
       <c r="A357" s="2" t="n">
@@ -17582,11 +15801,6 @@
           <t>GÖKDERE MAHALLESİ CEYLAN SOKAK NO:9/B BORNOVA / İZMİR</t>
         </is>
       </c>
-      <c r="J357" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="358">
       <c r="A358" s="2" t="n">
@@ -17630,11 +15844,6 @@
           <t>CUMHURİYET MAHALLESİ TEMELPAŞA CAD. NO:40 GÜMÜLDÜR / İZMİR</t>
         </is>
       </c>
-      <c r="J358" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="359">
       <c r="A359" s="2" t="n">
@@ -17678,11 +15887,6 @@
           <t>MENDERES MAH. 1114 SK. NO: 6 İÇ KAPI NO: 2 GAZİEMİR / İZMİR</t>
         </is>
       </c>
-      <c r="J359" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="360">
       <c r="A360" s="2" t="n">
@@ -17726,11 +15930,6 @@
           <t>ZAFER MAHALLESİ TURGUT ÖZAL CAD. NO: 110 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J360" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="361">
       <c r="A361" s="2" t="n">
@@ -17774,11 +15973,6 @@
           <t>29 EKİM MAH. ATATÜRK CAD. NO: 239V İÇ KAPI NO: 13 BUCA / İZMİR</t>
         </is>
       </c>
-      <c r="J361" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="362">
       <c r="A362" s="2" t="n">
@@ -17822,11 +16016,6 @@
           <t>ALSANCAK MAHALLESİ 1473 SOKAK NO:5/608 KONAK / İZMİR</t>
         </is>
       </c>
-      <c r="J362" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="363">
       <c r="A363" s="2" t="n">
@@ -17870,11 +16059,6 @@
           <t>TEPECİK MAHALLESİ KUŞADASI CAD. UÇAK KARDEŞLER BLOK NO: 79A SEFERİHİSAR / İZMİR</t>
         </is>
       </c>
-      <c r="J363" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="364">
       <c r="A364" s="2" t="n">
@@ -17918,11 +16102,6 @@
           <t>MERİÇ MAHALLESİ 5747/3 SK. NO: 1/1 BORNOVA/İZMİR</t>
         </is>
       </c>
-      <c r="J364" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
-        </is>
-      </c>
     </row>
     <row r="365">
       <c r="A365" s="2" t="n">
@@ -17964,11 +16143,6 @@
       <c r="I365" s="2" t="inlineStr">
         <is>
           <t>ÇORAKKAPI MAHALLESİ MÜRSELPAŞA BULV. NO:24 ASLANBEY İŞHANI KAT:7 DAİRE:14 KONAK/İZMİR</t>
-        </is>
-      </c>
-      <c r="J365" s="2" t="inlineStr">
-        <is>
-          <t>01 - YAŞ SEBZE MEYVE GRUBU</t>
         </is>
       </c>
     </row>

</xml_diff>